<commit_message>
Added results on job quality
</commit_message>
<xml_diff>
--- a/Results/table_individuals.xlsx
+++ b/Results/table_individuals.xlsx
@@ -391,10 +391,10 @@
         </is>
       </c>
       <c r="C2">
-        <v>15819</v>
+        <v>15816</v>
       </c>
       <c r="D2">
-        <v>0.4391848746494905</v>
+        <v>0.4392357253943568</v>
       </c>
     </row>
     <row r="3">
@@ -409,10 +409,10 @@
         </is>
       </c>
       <c r="C3">
-        <v>20200</v>
+        <v>20192</v>
       </c>
       <c r="D3">
-        <v>0.5608151253505095</v>
+        <v>0.5607642746056432</v>
       </c>
     </row>
     <row r="4">
@@ -427,10 +427,10 @@
         </is>
       </c>
       <c r="C4">
-        <v>24588</v>
+        <v>24584</v>
       </c>
       <c r="D4">
-        <v>0.6826397179266498</v>
+        <v>0.6827371695178849</v>
       </c>
     </row>
     <row r="5">
@@ -445,10 +445,10 @@
         </is>
       </c>
       <c r="C5">
-        <v>6947</v>
+        <v>6941</v>
       </c>
       <c r="D5">
-        <v>0.192870429495544</v>
+        <v>0.1927627193956898</v>
       </c>
     </row>
     <row r="6">
@@ -463,10 +463,10 @@
         </is>
       </c>
       <c r="C6">
-        <v>4484</v>
+        <v>4483</v>
       </c>
       <c r="D6">
-        <v>0.1244898525778062</v>
+        <v>0.1245001110864252</v>
       </c>
     </row>
     <row r="7">
@@ -481,10 +481,10 @@
         </is>
       </c>
       <c r="C7">
-        <v>10709</v>
+        <v>10706</v>
       </c>
       <c r="D7">
-        <v>0.2973153058108221</v>
+        <v>0.2973228171517441</v>
       </c>
     </row>
     <row r="8">
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="C8">
-        <v>18433</v>
+        <v>18426</v>
       </c>
       <c r="D8">
-        <v>0.5117576834448485</v>
+        <v>0.5117196178626972</v>
       </c>
     </row>
     <row r="9">
@@ -517,10 +517,10 @@
         </is>
       </c>
       <c r="C9">
-        <v>6877</v>
+        <v>6876</v>
       </c>
       <c r="D9">
-        <v>0.1909270107443294</v>
+        <v>0.1909575649855588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>